<commit_message>
Upload and scan agency_id
Upload and scan agency_id for single row
</commit_message>
<xml_diff>
--- a/Use this.xlsx
+++ b/Use this.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tohme\Documents\Documents\SP\Accenture\ADES\code\Hui shi excel to database\Upoad-excel-data-to-database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67710447-FCD3-4011-B375-C7C8E4878C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F7CB2E3-7347-4CA3-8EF7-F94532FA2968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{ED30F97F-71D3-448D-A260-C1EE2D5B2285}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="93">
   <si>
     <t>Agency</t>
   </si>
@@ -313,6 +313,10 @@
   </si>
   <si>
     <t xml:space="preserve">WSH EXPERTS PTE. LTD.
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">530320.00,
 </t>
   </si>
 </sst>
@@ -696,7 +700,7 @@
   <dimension ref="A1:BN6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AV1" workbookViewId="0">
-      <selection activeCell="BG9" sqref="BG9"/>
+      <selection activeCell="BH15" sqref="BH15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1111,6 +1115,9 @@
       </c>
       <c r="BH2" t="s">
         <v>91</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>92</v>
       </c>
       <c r="BJ2" t="s">
         <v>73</v>

</xml_diff>